<commit_message>
Correção dos artefatos para ac 05
</commit_message>
<xml_diff>
--- a/Artefatos/17. Análise dos Eventos para cada Cenário.xlsx
+++ b/Artefatos/17. Análise dos Eventos para cada Cenário.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
   <si>
     <t>Externo</t>
   </si>
@@ -106,10 +106,34 @@
     <t>Cliente solicita acompanhamento</t>
   </si>
   <si>
+    <t>Atendente recebe ficha técnica</t>
+  </si>
+  <si>
+    <t>X(11)</t>
+  </si>
+  <si>
+    <t>Cliente recebe rotina nutricional</t>
+  </si>
+  <si>
+    <t>X(12)</t>
+  </si>
+  <si>
+    <t>Preparador físico envia desafios</t>
+  </si>
+  <si>
+    <t>Cliente recebe desafios</t>
+  </si>
+  <si>
+    <t>X(14)</t>
+  </si>
+  <si>
+    <t>Cliente conclui desafios</t>
+  </si>
+  <si>
+    <t>X(15)</t>
+  </si>
+  <si>
     <t>Cliente cancela acompanhamento</t>
-  </si>
-  <si>
-    <t>X(11)</t>
   </si>
 </sst>
 </file>
@@ -254,7 +278,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -306,10 +330,7 @@
     <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" textRotation="90"/>
     </xf>
-    <xf borderId="0" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" textRotation="90"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="8" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -776,9 +797,6 @@
       <c r="J13" s="11"/>
     </row>
     <row r="14" ht="37.5" customHeight="1">
-      <c r="B14" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="C14" s="1">
         <v>12.0</v>
       </c>
@@ -795,22 +813,93 @@
       <c r="J14" s="11"/>
     </row>
     <row r="15">
-      <c r="A15" s="19"/>
-      <c r="E15" s="20"/>
+      <c r="C15" s="1">
+        <v>13.0</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="16"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="11"/>
     </row>
     <row r="16">
-      <c r="A16" s="19"/>
+      <c r="C16" s="1">
+        <v>14.0</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" s="16"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="11"/>
     </row>
     <row r="17">
-      <c r="A17" s="19"/>
+      <c r="C17" s="1">
+        <v>15.0</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" s="16"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="11"/>
     </row>
     <row r="18">
-      <c r="A18" s="19"/>
+      <c r="C18" s="1">
+        <v>16.0</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" s="16"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="11"/>
+    </row>
+    <row r="19">
+      <c r="B19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="1">
+        <v>17.0</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="8"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="J19" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="A7:A12"/>
-    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A13:A19"/>
+    <mergeCell ref="B13:B18"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="A2:B2"/>

</xml_diff>

<commit_message>
Correção dos artefatos para a prova final
</commit_message>
<xml_diff>
--- a/Artefatos/17. Análise dos Eventos para cada Cenário.xlsx
+++ b/Artefatos/17. Análise dos Eventos para cada Cenário.xlsx
@@ -94,7 +94,7 @@
     <t>Cliente altera pedido</t>
   </si>
   <si>
-    <t>Atendente recebe recusa do produto</t>
+    <t>Cliente recusa produto</t>
   </si>
   <si>
     <t>X(7)</t>
@@ -112,7 +112,7 @@
     <t>X(11)</t>
   </si>
   <si>
-    <t>Cliente recebe rotina nutricional</t>
+    <t>Cliente envia rotina nutricional</t>
   </si>
   <si>
     <t>X(12)</t>
@@ -278,7 +278,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -326,6 +326,15 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" textRotation="90"/>
@@ -762,20 +771,20 @@
       <c r="C12" s="1">
         <v>10.0</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="18" t="s">
         <v>27</v>
       </c>
       <c r="E12" s="8"/>
-      <c r="F12" s="16"/>
+      <c r="F12" s="19" t="s">
+        <v>28</v>
+      </c>
       <c r="G12" s="9"/>
-      <c r="H12" s="9" t="s">
-        <v>28</v>
-      </c>
+      <c r="H12" s="20"/>
       <c r="I12" s="9"/>
       <c r="J12" s="11"/>
     </row>
     <row r="13" ht="36.0" customHeight="1">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="21" t="s">
         <v>29</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -816,7 +825,7 @@
       <c r="C15" s="1">
         <v>13.0</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="18" t="s">
         <v>33</v>
       </c>
       <c r="E15" s="8" t="s">
@@ -832,7 +841,7 @@
       <c r="C16" s="1">
         <v>14.0</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="22" t="s">
         <v>35</v>
       </c>
       <c r="E16" s="8" t="s">

</xml_diff>